<commit_message>
Added elegant handling of invalid settings ready for v2.0
</commit_message>
<xml_diff>
--- a/assets/downloads/AppSettingsGenerator.xlsx
+++ b/assets/downloads/AppSettingsGenerator.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/upnrunning/drive/otherdev/mailchimp-mailshot-sync/assets/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0135DFAB-AC5A-F24D-A978-9F2C566285CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B967BD6-DFE5-9249-9DAD-CB8A2DE48E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="28040" windowHeight="16560" activeTab="2" xr2:uid="{8C62FFF8-0907-C849-B338-22CB3978E440}"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{8C62FFF8-0907-C849-B338-22CB3978E440}"/>
   </bookViews>
   <sheets>
     <sheet name="Zendesk User Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Hidden" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -447,17 +447,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="5"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -467,6 +458,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -478,67 +478,7 @@
     <cellStyle name="Note" xfId="6" builtinId="10"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -930,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6472FB2-45C1-434B-B660-46CD8D84B706}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,17 +889,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="366" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12" t="str">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9" t="str">
         <f>CONCATENATE("[",CHAR(10),$O$3, $O$4, $O$5, $O$6, $O$7, $O$8, $O$9, $O$10, $O$11, $O$12, $O$13, $O$314, $O$15, $O$16, $O$17,"]")</f>
         <v>[
   {
@@ -978,8 +918,8 @@
   }
 ]</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:16" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1032,10 +972,10 @@
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1045,14 +985,14 @@
         <v>4</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="str">
         <f>TRIM(MID(SUBSTITUTE($G3,"|",REPT(" ",LEN($G3))),(1-1)*LEN($G3)+1,LEN($G3)))</f>
         <v>TRUE</v>
       </c>
-      <c r="I3" s="8" t="str">
+      <c r="I3" s="6" t="str">
         <f>TRIM(MID(SUBSTITUTE($G3,"|",REPT(" ",LEN($G3))),(2-1)*LEN($G3)+1,LEN($G3)))</f>
         <v>text</v>
       </c>
@@ -1085,8 +1025,8 @@
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1094,14 +1034,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ref="H4:H17" si="0">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(1-1)*LEN($G4)+1,LEN($G4)))</f>
         <v>TRUE</v>
       </c>
-      <c r="I4" s="8" t="str">
+      <c r="I4" s="6" t="str">
         <f t="shared" ref="I4:I17" si="1">TRIM(MID(SUBSTITUTE($G4,"|",REPT(" ",LEN($G4))),(2-1)*LEN($G4)+1,LEN($G4)))</f>
         <v>text</v>
       </c>
@@ -1155,7 +1095,7 @@
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I5" s="8" t="str">
+      <c r="I5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>text</v>
       </c>
@@ -1211,7 +1151,7 @@
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I6" s="8" t="str">
+      <c r="I6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>number</v>
       </c>
@@ -1276,7 +1216,7 @@
         <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
-      <c r="I7" s="8" t="str">
+      <c r="I7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>text</v>
       </c>
@@ -1341,7 +1281,7 @@
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="I8" s="8" t="str">
+      <c r="I8" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1399,7 +1339,7 @@
         <f t="shared" si="0"/>
         <v>FALSE</v>
       </c>
-      <c r="I9" s="8" t="str">
+      <c r="I9" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1447,7 +1387,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I10" s="8" t="str">
+      <c r="I10" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1495,7 +1435,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I11" s="8" t="str">
+      <c r="I11" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1543,7 +1483,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I12" s="8" t="str">
+      <c r="I12" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1591,7 +1531,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I13" s="8" t="str">
+      <c r="I13" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1639,7 +1579,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I14" s="8" t="str">
+      <c r="I14" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1687,7 +1627,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I15" s="8" t="str">
+      <c r="I15" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1735,7 +1675,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I16" s="8" t="str">
+      <c r="I16" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1783,7 +1723,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I17" s="8" t="str">
+      <c r="I17" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -1830,13 +1770,13 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K17">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(($H3="TRUE"), $J3="")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(($H3="TRUE"), $J3&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>($H3="FALSE")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1887,7 +1827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9F628A-5B28-144E-A295-0A4EE9D4CFF1}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1936,84 +1876,84 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2021,114 +1961,114 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>